<commit_message>
Fix validation test bug
</commit_message>
<xml_diff>
--- a/openn/tests/data/diaries/ism/openn_metadata.xlsx
+++ b/openn/tests/data/diaries/ism/openn_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeryr/code/GIT/openn/openn/tests/data/diaries/ism/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,6 @@
     <sheet name="VALUE LISTS" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -68,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="3979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4411" uniqueCount="3979">
   <si>
     <t>1r</t>
   </si>
@@ -13691,10 +13690,10 @@
   <dimension ref="A1:L196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15155,7 +15154,9 @@
       <c r="D68" t="s">
         <v>3787</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F68" s="15" t="s">
         <v>3788</v>
       </c>
@@ -15176,7 +15177,9 @@
       <c r="D69" t="s">
         <v>3789</v>
       </c>
-      <c r="E69" s="2"/>
+      <c r="E69" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F69" s="15" t="s">
         <v>3790</v>
       </c>
@@ -15197,7 +15200,9 @@
       <c r="D70" t="s">
         <v>3791</v>
       </c>
-      <c r="E70" s="2"/>
+      <c r="E70" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F70" s="15" t="s">
         <v>3792</v>
       </c>
@@ -15218,7 +15223,9 @@
       <c r="D71" t="s">
         <v>3793</v>
       </c>
-      <c r="E71" s="2"/>
+      <c r="E71" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F71" s="15" t="s">
         <v>3794</v>
       </c>
@@ -15239,7 +15246,9 @@
       <c r="D72" t="s">
         <v>3795</v>
       </c>
-      <c r="E72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F72" s="15" t="s">
         <v>3796</v>
       </c>
@@ -15260,7 +15269,9 @@
       <c r="D73" t="s">
         <v>3797</v>
       </c>
-      <c r="E73" s="2"/>
+      <c r="E73" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F73" s="15" t="s">
         <v>3798</v>
       </c>
@@ -15281,7 +15292,9 @@
       <c r="D74" t="s">
         <v>3799</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F74" s="15" t="s">
         <v>3800</v>
       </c>
@@ -15302,7 +15315,9 @@
       <c r="D75" t="s">
         <v>3801</v>
       </c>
-      <c r="E75" s="2"/>
+      <c r="E75" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F75" s="15" t="s">
         <v>3802</v>
       </c>
@@ -15323,7 +15338,9 @@
       <c r="D76" t="s">
         <v>3803</v>
       </c>
-      <c r="E76" s="2"/>
+      <c r="E76" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F76" s="15" t="s">
         <v>3804</v>
       </c>
@@ -15344,7 +15361,9 @@
       <c r="D77" t="s">
         <v>3805</v>
       </c>
-      <c r="E77" s="2"/>
+      <c r="E77" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F77" s="15" t="s">
         <v>3806</v>
       </c>
@@ -15384,7 +15403,9 @@
       <c r="D79" t="s">
         <v>3808</v>
       </c>
-      <c r="E79" s="2"/>
+      <c r="E79" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F79" s="15" t="s">
         <v>3809</v>
       </c>
@@ -15405,7 +15426,9 @@
       <c r="D80" t="s">
         <v>3810</v>
       </c>
-      <c r="E80" s="2"/>
+      <c r="E80" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F80" s="15" t="s">
         <v>3811</v>
       </c>
@@ -15426,7 +15449,9 @@
       <c r="D81" t="s">
         <v>3812</v>
       </c>
-      <c r="E81" s="2"/>
+      <c r="E81" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F81" s="15" t="s">
         <v>3813</v>
       </c>
@@ -15447,7 +15472,9 @@
       <c r="D82" t="s">
         <v>3814</v>
       </c>
-      <c r="E82" s="2"/>
+      <c r="E82" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F82" s="15" t="s">
         <v>3815</v>
       </c>
@@ -15468,7 +15495,9 @@
       <c r="D83" t="s">
         <v>3816</v>
       </c>
-      <c r="E83" s="2"/>
+      <c r="E83" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F83" s="15" t="s">
         <v>3817</v>
       </c>
@@ -15508,7 +15537,9 @@
       <c r="D85" t="s">
         <v>3819</v>
       </c>
-      <c r="E85" s="2"/>
+      <c r="E85" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F85" s="15" t="s">
         <v>3820</v>
       </c>
@@ -15529,7 +15560,9 @@
       <c r="D86" t="s">
         <v>3821</v>
       </c>
-      <c r="E86" s="2"/>
+      <c r="E86" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F86" s="15" t="s">
         <v>3822</v>
       </c>
@@ -15550,7 +15583,9 @@
       <c r="D87" t="s">
         <v>3823</v>
       </c>
-      <c r="E87" s="2"/>
+      <c r="E87" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F87" s="15" t="s">
         <v>3824</v>
       </c>
@@ -15571,7 +15606,9 @@
       <c r="D88" t="s">
         <v>3825</v>
       </c>
-      <c r="E88" s="2"/>
+      <c r="E88" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F88" s="15" t="s">
         <v>3826</v>
       </c>
@@ -15592,7 +15629,9 @@
       <c r="D89" t="s">
         <v>3827</v>
       </c>
-      <c r="E89" s="2"/>
+      <c r="E89" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F89" s="15" t="s">
         <v>3828</v>
       </c>
@@ -15613,7 +15652,9 @@
       <c r="D90" t="s">
         <v>3829</v>
       </c>
-      <c r="E90" s="2"/>
+      <c r="E90" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F90" s="15" t="s">
         <v>3830</v>
       </c>
@@ -15634,7 +15675,9 @@
       <c r="D91" t="s">
         <v>3831</v>
       </c>
-      <c r="E91" s="2"/>
+      <c r="E91" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F91" s="15" t="s">
         <v>3832</v>
       </c>
@@ -15655,7 +15698,9 @@
       <c r="D92" t="s">
         <v>3833</v>
       </c>
-      <c r="E92" s="2"/>
+      <c r="E92" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F92" s="15" t="s">
         <v>3834</v>
       </c>
@@ -15676,7 +15721,9 @@
       <c r="D93" t="s">
         <v>3835</v>
       </c>
-      <c r="E93" s="2"/>
+      <c r="E93" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F93" s="15" t="s">
         <v>3836</v>
       </c>
@@ -15697,7 +15744,9 @@
       <c r="D94" t="s">
         <v>3837</v>
       </c>
-      <c r="E94" s="2"/>
+      <c r="E94" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F94" s="15" t="s">
         <v>3838</v>
       </c>
@@ -15718,7 +15767,9 @@
       <c r="D95" t="s">
         <v>3839</v>
       </c>
-      <c r="E95" s="2"/>
+      <c r="E95" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F95" s="15" t="s">
         <v>3840</v>
       </c>
@@ -15739,7 +15790,9 @@
       <c r="D96" t="s">
         <v>3841</v>
       </c>
-      <c r="E96" s="2"/>
+      <c r="E96" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F96" s="15" t="s">
         <v>3842</v>
       </c>
@@ -15760,7 +15813,9 @@
       <c r="D97" t="s">
         <v>3843</v>
       </c>
-      <c r="E97" s="2"/>
+      <c r="E97" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F97" s="15" t="s">
         <v>3844</v>
       </c>
@@ -15781,7 +15836,9 @@
       <c r="D98" t="s">
         <v>3845</v>
       </c>
-      <c r="E98" s="2"/>
+      <c r="E98" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F98" s="15" t="s">
         <v>3846</v>
       </c>
@@ -15802,7 +15859,9 @@
       <c r="D99" t="s">
         <v>3847</v>
       </c>
-      <c r="E99" s="2"/>
+      <c r="E99" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F99" s="15" t="s">
         <v>3848</v>
       </c>
@@ -15842,7 +15901,9 @@
       <c r="D101" t="s">
         <v>3850</v>
       </c>
-      <c r="E101" s="2"/>
+      <c r="E101" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F101" s="15" t="s">
         <v>3851</v>
       </c>
@@ -15996,7 +16057,9 @@
       <c r="D109" t="s">
         <v>3859</v>
       </c>
-      <c r="E109" s="2"/>
+      <c r="E109" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F109" s="15" t="s">
         <v>3860</v>
       </c>
@@ -16017,7 +16080,9 @@
       <c r="D110" t="s">
         <v>3861</v>
       </c>
-      <c r="E110" s="2"/>
+      <c r="E110" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F110" s="15" t="s">
         <v>3862</v>
       </c>
@@ -16038,7 +16103,9 @@
       <c r="D111" t="s">
         <v>3863</v>
       </c>
-      <c r="E111" s="2"/>
+      <c r="E111" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F111" s="15" t="s">
         <v>3864</v>
       </c>
@@ -16059,7 +16126,9 @@
       <c r="D112" t="s">
         <v>3865</v>
       </c>
-      <c r="E112" s="2"/>
+      <c r="E112" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F112" s="15" t="s">
         <v>3866</v>
       </c>
@@ -16080,7 +16149,9 @@
       <c r="D113" t="s">
         <v>3867</v>
       </c>
-      <c r="E113" s="2"/>
+      <c r="E113" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F113" s="15" t="s">
         <v>3868</v>
       </c>
@@ -16120,7 +16191,9 @@
       <c r="D115" t="s">
         <v>3870</v>
       </c>
-      <c r="E115" s="2"/>
+      <c r="E115" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F115" s="15" t="s">
         <v>3871</v>
       </c>
@@ -16160,7 +16233,9 @@
       <c r="D117" t="s">
         <v>3873</v>
       </c>
-      <c r="E117" s="2"/>
+      <c r="E117" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F117" s="15" t="s">
         <v>3874</v>
       </c>
@@ -16221,7 +16296,9 @@
       <c r="D120" t="s">
         <v>3877</v>
       </c>
-      <c r="E120" s="2"/>
+      <c r="E120" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F120" s="15" t="s">
         <v>3878</v>
       </c>
@@ -16451,7 +16528,9 @@
       <c r="D132" t="s">
         <v>3890</v>
       </c>
-      <c r="E132" s="2"/>
+      <c r="E132" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F132" s="15" t="s">
         <v>3891</v>
       </c>
@@ -16472,7 +16551,9 @@
       <c r="D133" t="s">
         <v>3892</v>
       </c>
-      <c r="E133" s="2"/>
+      <c r="E133" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F133" s="15" t="s">
         <v>3891</v>
       </c>
@@ -16493,7 +16574,9 @@
       <c r="D134" t="s">
         <v>3893</v>
       </c>
-      <c r="E134" s="2"/>
+      <c r="E134" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F134" s="15" t="s">
         <v>3894</v>
       </c>
@@ -16514,7 +16597,9 @@
       <c r="D135" t="s">
         <v>3895</v>
       </c>
-      <c r="E135" s="2"/>
+      <c r="E135" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F135" s="15" t="s">
         <v>3896</v>
       </c>
@@ -16535,7 +16620,9 @@
       <c r="D136" t="s">
         <v>3897</v>
       </c>
-      <c r="E136" s="2"/>
+      <c r="E136" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F136" s="15" t="s">
         <v>3898</v>
       </c>
@@ -16575,7 +16662,9 @@
       <c r="D138" t="s">
         <v>3900</v>
       </c>
-      <c r="E138" s="2"/>
+      <c r="E138" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F138" s="15" t="s">
         <v>3901</v>
       </c>
@@ -16672,7 +16761,9 @@
       <c r="D143" t="s">
         <v>3906</v>
       </c>
-      <c r="E143" s="2"/>
+      <c r="E143" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F143" s="15" t="s">
         <v>3907</v>
       </c>
@@ -16693,7 +16784,9 @@
       <c r="D144" t="s">
         <v>3908</v>
       </c>
-      <c r="E144" s="2"/>
+      <c r="E144" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F144" s="15" t="s">
         <v>3909</v>
       </c>
@@ -16733,7 +16826,9 @@
       <c r="D146" t="s">
         <v>3911</v>
       </c>
-      <c r="E146" s="2"/>
+      <c r="E146" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F146" s="15" t="s">
         <v>3912</v>
       </c>
@@ -16811,7 +16906,9 @@
       <c r="D150" t="s">
         <v>3916</v>
       </c>
-      <c r="E150" s="2"/>
+      <c r="E150" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F150" s="15" t="s">
         <v>3917</v>
       </c>
@@ -16908,7 +17005,9 @@
       <c r="D155" t="s">
         <v>3922</v>
       </c>
-      <c r="E155" s="2"/>
+      <c r="E155" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F155" s="15" t="s">
         <v>3923</v>
       </c>
@@ -17480,7 +17579,9 @@
       <c r="D185" t="s">
         <v>3953</v>
       </c>
-      <c r="E185" s="2"/>
+      <c r="E185" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F185" s="15" t="s">
         <v>3954</v>
       </c>
@@ -17564,7 +17665,9 @@
       <c r="D189" t="s">
         <v>3958</v>
       </c>
-      <c r="E189" s="2"/>
+      <c r="E189" s="2" t="s">
+        <v>2617</v>
+      </c>
       <c r="F189" s="15" t="s">
         <v>3959</v>
       </c>

</xml_diff>